<commit_message>
Raw and Clean Data from SSA for June 3rd
</commit_message>
<xml_diff>
--- a/data-raw/base3.xlsx
+++ b/data-raw/base3.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-Data/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{314F139D-6503-3045-A3B1-2CA1E82D9B7A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D27281-6C14-7345-8308-66A3117E222D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="960" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
+    <workbookView xWindow="780" yWindow="480" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -199,7 +199,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3" applyAlignment="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="5" applyNumberFormat="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
@@ -228,6 +227,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,15 +575,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="64" x14ac:dyDescent="0.2">
@@ -593,7 +619,7 @@
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="6">
+      <c r="A2" s="15">
         <v>43983</v>
       </c>
       <c r="B2" s="5">
@@ -625,35 +651,67 @@
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="16">
+      <c r="A3" s="15">
         <v>43984</v>
       </c>
-      <c r="B3" s="7">
+      <c r="B3" s="6">
         <v>97326</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>153601</v>
       </c>
-      <c r="D3" s="9">
+      <c r="D3" s="8">
         <v>42151</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="9">
         <v>10637</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="10">
         <v>34.586852434087504</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="11">
         <v>33662</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="12">
         <v>3169</v>
       </c>
-      <c r="I3" s="14">
+      <c r="I3" s="13">
         <v>3342</v>
       </c>
-      <c r="J3" s="15">
+      <c r="J3" s="14">
         <v>293078</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="15">
+        <v>43985</v>
+      </c>
+      <c r="B4" s="16">
+        <v>101238</v>
+      </c>
+      <c r="C4" s="17">
+        <v>157354</v>
+      </c>
+      <c r="D4" s="18">
+        <v>44869</v>
+      </c>
+      <c r="E4" s="19">
+        <v>11728</v>
+      </c>
+      <c r="F4" s="20">
+        <v>34.450502775637602</v>
+      </c>
+      <c r="G4" s="21">
+        <v>34877</v>
+      </c>
+      <c r="H4" s="22">
+        <v>3293</v>
+      </c>
+      <c r="I4" s="23">
+        <v>3459</v>
+      </c>
+      <c r="J4" s="24">
+        <v>303461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Raw and Clean Data from SSA for June 4th
</commit_message>
<xml_diff>
--- a/data-raw/base3.xlsx
+++ b/data-raw/base3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marianafernandez/Documents/COSMO/covid19-mx-data/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68D27281-6C14-7345-8308-66A3117E222D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2D066F-A780-A94B-88F1-8F463443BAF8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="480" windowWidth="27640" windowHeight="16540" xr2:uid="{631A4B89-8883-AF43-AB16-93381ECA1B6C}"/>
   </bookViews>
@@ -184,7 +184,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -227,6 +227,33 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="2" applyNumberFormat="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3">
@@ -575,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5CC6AE2-E62C-4446-AE0C-06004275548D}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -714,6 +741,38 @@
         <v>303461</v>
       </c>
     </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="15">
+        <v>43986</v>
+      </c>
+      <c r="B5" s="25">
+        <v>105680</v>
+      </c>
+      <c r="C5" s="26">
+        <v>161724</v>
+      </c>
+      <c r="D5" s="27">
+        <v>46659</v>
+      </c>
+      <c r="E5" s="28">
+        <v>12545</v>
+      </c>
+      <c r="F5" s="29">
+        <v>34.235427706283119</v>
+      </c>
+      <c r="G5" s="30">
+        <v>36180</v>
+      </c>
+      <c r="H5" s="31">
+        <v>3405</v>
+      </c>
+      <c r="I5" s="32">
+        <v>3587</v>
+      </c>
+      <c r="J5" s="33">
+        <v>314063</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>